<commit_message>
Clean up generated code for recurrence-chained-20220730
</commit_message>
<xml_diff>
--- a/LoopGen/recurrence-chained-20220730/cores.xlsx
+++ b/LoopGen/recurrence-chained-20220730/cores.xlsx
@@ -458,9 +458,9 @@
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
     (*D)[i] = (*D)[i - 1];
-    (*B)[i] = (*B)[i - 1] + 0;
-    (*A)[i] = (*A)[i - 1] + 0;
-    (*C)[i] = (*C)[i - 1] + 0;
+    (*B)[i] = (*B)[i - 1];
+    (*A)[i] = (*A)[i - 1];
+    (*C)[i] = (*C)[i - 1];
   }
 </t>
         </is>
@@ -480,8 +480,8 @@
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
     (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
     (*D)[i] = (*D)[i - 1];
-    (*C)[i] = (*C)[i - 1] + 0;
-    (*B)[i] = (*B)[i - 1] + 0;
+    (*C)[i] = (*C)[i - 1];
+    (*B)[i] = (*B)[i - 1];
   }
 </t>
         </is>
@@ -499,7 +499,7 @@
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 1; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (*C)[i - 1] + 0;
+    (*C)[i] = (*C)[i - 1];
     (*A)[i] = (*A)[i - 1] + (*B)[i - 1];
     (*D)[i] = (*D)[i - 1];
     (*B)[i] = (*B)[i - 1] + (*C)[i - 1];
@@ -541,10 +541,10 @@
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + 0;
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*B)[i] = (*B)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = (*A)[i - 2];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -562,10 +562,10 @@
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + 0;
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + 0;
+    (*B)[i] = (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = (*A)[i - 1] + (*A)[i - 2];
   }
 </t>
         </is>
@@ -583,10 +583,10 @@
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + 0;
-    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*B)[i] = (*B)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = 2 * (*A)[i - 1] + (*A)[i - 2];
+    (*C)[i] = 2 * (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -604,9 +604,9 @@
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + 0;
+    (*B)[i] = (*B)[i - 2];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
+    (*A)[i] = (*A)[i - 1] + (*A)[i - 2];
     (*D)[i] = 2 * (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
@@ -625,9 +625,9 @@
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + 0;
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 2];
+    (*A)[i] = 2 * (*A)[i - 1] + (*A)[i - 2];
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
     (*D)[i] = 2 * (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
@@ -646,10 +646,10 @@
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -667,9 +667,9 @@
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + 0;
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
+    (*B)[i] = (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
     (*D)[i] = 2 * (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
@@ -688,10 +688,10 @@
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + 0;
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2];
+    (*A)[i] = (*A)[i - 2] + ((*B)[i - 1] + (*B)[i - 2]);
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -709,10 +709,10 @@
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + 0;
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*C)[i] = (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + ((*B)[i - 1] + (*B)[i - 2]);
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 2];
   }
 </t>
         </is>
@@ -730,10 +730,10 @@
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + ((*B)[i - 1] + (*B)[i - 2]);
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 2];
   }
 </t>
         </is>
@@ -751,9 +751,9 @@
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + 0;
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + 0;
+    (*C)[i] = 2 * (*C)[i - 1] + (*C)[i - 2];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
+    (*B)[i] = (*B)[i - 1] + (*B)[i - 2];
     (*D)[i] = 2 * (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
@@ -772,10 +772,10 @@
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*C)[i] = (*C)[i - 2];
   }
 </t>
         </is>
@@ -793,10 +793,10 @@
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
-    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*C)[i] = 2 * (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -814,10 +814,10 @@
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*A)[i] = (*A)[i - 2] + ((*B)[i - 1] + (*B)[i - 2]);
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -835,10 +835,10 @@
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
-    (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + ((*B)[i - 1] + (*B)[i - 2]);
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -856,10 +856,10 @@
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (2 * (*B)[i - 1] + (*B)[i - 2]);
     (*B)[i] = (2 * (*B)[i - 1] + (*B)[i - 2]) + (2 * (*C)[i - 1] + (*C)[i - 2]);
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*C)[i] = (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -877,10 +877,10 @@
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + (1 * (*C)[i - 1] + (*C)[i - 2]);
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + ((*C)[i - 1] + (*C)[i - 2]);
     (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*C)[i] = 2 * (*C)[i - 1] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -898,10 +898,10 @@
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + 0;
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + ((*B)[i - 1] + (*B)[i - 2]);
+    (*C)[i] = 2 * (*C)[i - 1] + (*C)[i - 2];
     (*B)[i] = (2 * (*B)[i - 1] + (*B)[i - 2]) + (2 * (*C)[i - 1] + (*C)[i - 2]);
-    (*D)[i] = 1 * (*D)[i - 1] + (*D)[i - 2];
+    (*D)[i] = (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
         </is>
@@ -919,10 +919,10 @@
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + (0 * (*D)[i - 1] + (*D)[i - 2]);
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2] + (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
   }
 </t>
         </is>
@@ -940,10 +940,10 @@
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + (0 * (*D)[i - 1] + (*D)[i - 2]);
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (2 * (*C)[i - 1] + (*C)[i - 2]);
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*C)[i] = (*C)[i - 2] + (*D)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*B)[i] = (*B)[i - 2] + (2 * (*C)[i - 1] + (*C)[i - 2]);
   }
 </t>
         </is>
@@ -961,10 +961,10 @@
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + (0 * (*D)[i - 1] + (*D)[i - 2]);
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (0 * (*A)[i - 1] + (*A)[i - 2]) + (0 * (*B)[i - 1] + (*B)[i - 2]);
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + (1 * (*C)[i - 1] + (*C)[i - 2]);
+    (*C)[i] = (*C)[i - 2] + (*D)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = (*A)[i - 2] + (*B)[i - 2];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + ((*C)[i - 1] + (*C)[i - 2]);
   }
 </t>
         </is>
@@ -982,10 +982,10 @@
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + (0 * (*D)[i - 1] + (*D)[i - 2]);
-    (*D)[i] = 1 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*C)[i] = (*C)[i - 2] + (*D)[i - 2];
+    (*D)[i] = (*D)[i - 1] + (*D)[i - 2];
+    (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + ((*B)[i - 1] + (*B)[i - 2]);
   }
 </t>
         </is>
@@ -1003,10 +1003,10 @@
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (0 * (*C)[i - 1] + (*C)[i - 2]) + (0 * (*D)[i - 1] + (*D)[i - 2]);
-    (*D)[i] = 0 * (*D)[i - 1] + (*D)[i - 2];
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + (1 * (*C)[i - 1] + (*C)[i - 2]);
+    (*C)[i] = (*C)[i - 2] + (*D)[i - 2];
+    (*D)[i] = (*D)[i - 2];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + ((*C)[i - 1] + (*C)[i - 2]);
   }
 </t>
         </is>
@@ -1024,10 +1024,10 @@
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (0 * (*C)[i - 1] + (*C)[i - 2]);
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + (2 * (*D)[i - 1] + (*D)[i - 2]);
+    (*B)[i] = (*B)[i - 2] + (*C)[i - 2];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 2]) + (2 * (*D)[i - 1] + (*D)[i - 2]);
     (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
-    (*D)[i] = 1 * (*D)[i - 1] + (*D)[i - 2];
+    (*D)[i] = (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
         </is>
@@ -1045,10 +1045,10 @@
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = (0 * (*B)[i - 1] + (*B)[i - 2]) + (2 * (*C)[i - 1] + (*C)[i - 2]);
+    (*B)[i] = (*B)[i - 2] + (2 * (*C)[i - 1] + (*C)[i - 2]);
     (*A)[i] = (2 * (*A)[i - 1] + (*A)[i - 2]) + (2 * (*B)[i - 1] + (*B)[i - 2]);
-    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + (1 * (*D)[i - 1] + (*D)[i - 2]);
-    (*D)[i] = 1 * (*D)[i - 1] + (*D)[i - 2];
+    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + ((*D)[i - 1] + (*D)[i - 2]);
+    (*D)[i] = (*D)[i - 1] + (*D)[i - 2];
   }
 </t>
         </is>
@@ -1066,10 +1066,10 @@
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 2; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = (1 * (*C)[i - 1] + (*C)[i - 2]) + (1 * (*D)[i - 1] + (*D)[i - 2]);
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 2]) + ((*D)[i - 1] + (*D)[i - 2]);
     (*D)[i] = 2 * (*D)[i - 1] + (*D)[i - 2];
-    (*B)[i] = (1 * (*B)[i - 1] + (*B)[i - 2]) + (1 * (*C)[i - 1] + (*C)[i - 2]);
-    (*A)[i] = (1 * (*A)[i - 1] + (*A)[i - 2]) + (1 * (*B)[i - 1] + (*B)[i - 2]);
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + ((*C)[i - 1] + (*C)[i - 2]);
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + ((*B)[i - 1] + (*B)[i - 2]);
   }
 </t>
         </is>
@@ -1087,10 +1087,10 @@
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*D)[i] = (*D)[i - 3];
   }
 </t>
         </is>
@@ -1108,10 +1108,10 @@
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
+    (*C)[i] = (*C)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3];
+    (*B)[i] = 2 * (*B)[i - 2] + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1129,10 +1129,10 @@
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
+    (*A)[i] = (*A)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1150,10 +1150,10 @@
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*A)[i] = ((0 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*A)[i] = (*A)[i - 2] + (*A)[i - 3];
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1171,10 +1171,10 @@
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((1 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*B)[i] = ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
+    (*C)[i] = (*C)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = ((*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3];
+    (*B)[i] = (2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1192,10 +1192,10 @@
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*C)[i] = ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*A)[i] = (*A)[i - 3];
+    (*D)[i] = (*D)[i - 2] + (*D)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3];
+    (*C)[i] = (2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1213,10 +1213,10 @@
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*A)[i] = ((1 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
+    (*D)[i] = (*D)[i - 3];
+    (*C)[i] = ((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3];
+    (*A)[i] = ((*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3];
   }
 </t>
         </is>
@@ -1234,10 +1234,10 @@
       <c r="C39" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((1 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
+    (*C)[i] = (*C)[i - 2] + (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3];
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*A)[i] = ((*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3];
   }
 </t>
         </is>
@@ -1255,10 +1255,10 @@
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + 0;
-    (*D)[i] = (1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*C)[i] = ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*A)[i] = (2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3];
+    (*D)[i] = ((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
+    (*B)[i] = (2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3];
+    (*C)[i] = ((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1276,10 +1276,10 @@
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*D)[i] = (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1297,10 +1297,10 @@
       <c r="C42" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (2 * (*B)[i - 2] + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1318,10 +1318,10 @@
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (2 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*D)[i] = (2 * (*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1339,10 +1339,10 @@
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*B)[i] = (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (2 * (*A)[i - 2] + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1360,10 +1360,10 @@
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*B)[i] = (*B)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1381,10 +1381,10 @@
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*A)[i] = ((0 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*A)[i] = (2 * (*A)[i - 2] + (*A)[i - 3]) + (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1402,10 +1402,10 @@
       <c r="C47" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3];
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1423,10 +1423,10 @@
       <c r="C48" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (2 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
+    (*A)[i] = (*A)[i - 3] + ((*B)[i - 2] + (*B)[i - 3]);
+    (*C)[i] = (2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3];
+    (*D)[i] = (2 * (*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1444,10 +1444,10 @@
       <c r="C49" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*C)[i] = (*C)[i - 3];
     (*D)[i] = (2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*B)[i] = (2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1465,10 +1465,10 @@
       <c r="C50" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
+    (*D)[i] = (*D)[i - 2] + (*D)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3];
   }
 </t>
         </is>
@@ -1486,9 +1486,9 @@
       <c r="C51" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((1 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + 0;
+    (*A)[i] = (((*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
+    (*B)[i] = ((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3];
     (*D)[i] = (2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
@@ -1507,10 +1507,10 @@
       <c r="C52" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*D)[i] = (*D)[i - 3];
   }
 </t>
         </is>
@@ -1528,10 +1528,10 @@
       <c r="C53" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (*C)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3] + ((*B)[i - 2] + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1549,10 +1549,10 @@
       <c r="C54" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*D)[i] = ((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1570,10 +1570,10 @@
       <c r="C55" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*B)[i] = (*B)[i - 3] + ((*C)[i - 2] + (*C)[i - 3]);
+    (*C)[i] = ((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1591,10 +1591,10 @@
       <c r="C56" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*D)[i] = (*D)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3] + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1612,10 +1612,10 @@
       <c r="C57" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((0 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*B)[i] = (2 * (*B)[i - 2] + (*B)[i - 3]) + ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]);
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1633,10 +1633,10 @@
       <c r="C58" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*B)[i] = ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*C)[i] = (2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1654,10 +1654,10 @@
       <c r="C59" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*C)[i] = (*C)[i - 3];
+    (*B)[i] = (*B)[i - 3] + ((*C)[i - 2] + (*C)[i - 3]);
     (*D)[i] = (2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1675,10 +1675,10 @@
       <c r="C60" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*D)[i] = (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*B)[i] = (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -1696,10 +1696,10 @@
       <c r="C61" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*B)[i] = (*B)[i - 3] + ((*C)[i - 2] + (*C)[i - 3]);
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1717,10 +1717,10 @@
       <c r="C62" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((1 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
+    (*B)[i] = (*B)[i - 3] + (((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]);
+    (*A)[i] = (((*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3];
   }
 </t>
         </is>
@@ -1738,10 +1738,10 @@
       <c r="C63" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = 2 * (*C)[i - 2] + (*C)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*B)[i] = (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]) + (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1759,10 +1759,10 @@
       <c r="C64" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + 0;
-    (*D)[i] = (2 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = ((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3];
+    (*D)[i] = (2 * (*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*B)[i] = (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -1780,10 +1780,10 @@
       <c r="C65" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*D)[i] = (*D)[i - 3];
   }
 </t>
         </is>
@@ -1801,10 +1801,10 @@
       <c r="C66" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (2 * (*B)[i - 2] + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -1822,10 +1822,10 @@
       <c r="C67" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
   }
 </t>
         </is>
@@ -1843,10 +1843,10 @@
       <c r="C68" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((0 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*B)[i] = (2 * (*B)[i - 2] + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -1864,10 +1864,10 @@
       <c r="C69" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*D)[i] = (*D)[i - 3];
+    (*B)[i] = ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]) + (((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -1885,10 +1885,10 @@
       <c r="C70" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((0 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*B)[i] = ((*B)[i - 2] + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1906,10 +1906,10 @@
       <c r="C71" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*D)[i] = (2 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*B)[i] = (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*D)[i] = (2 * (*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>
         </is>
@@ -1927,10 +1927,10 @@
       <c r="C72" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((0 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + ((2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*B)[i] = ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + (*B)[i - 3];
+    (*C)[i] = ((*C)[i - 2] + (*C)[i - 3]) + ((2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*B)[i] = (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -1948,10 +1948,10 @@
       <c r="C73" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]) + ((0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*D)[i] = (*D)[i - 3];
+    (*C)[i] = (*C)[i - 3] + (*D)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*B)[i] = ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]) + (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -1969,10 +1969,10 @@
       <c r="C74" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*D)[i] = (0 * (*D)[i - 1] + 0 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((0 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*B)[i] = ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + ((1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*D)[i] = (*D)[i - 3];
+    (*A)[i] = (*A)[i - 3] + ((*B)[i - 2] + (*B)[i - 3]);
+    (*B)[i] = ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]);
+    (*C)[i] = ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]) + (((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3]);
   }
 </t>
         </is>
@@ -1990,10 +1990,10 @@
       <c r="C75" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 0 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + ((1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*B)[i] = (*B)[i - 3] + (*C)[i - 3];
+    (*C)[i] = ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]) + (((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
   }
 </t>
         </is>
@@ -2011,10 +2011,10 @@
       <c r="C76" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((0 * (*B)[i - 1] + 0 * (*B)[i - 2]) + (*B)[i - 3]) + ((0 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((1 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((1 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + ((2 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*B)[i] = (*B)[i - 3] + ((*C)[i - 2] + (*C)[i - 3]);
+    (*A)[i] = ((2 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + (((*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (((*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]) + ((2 * (*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3]);
   }
 </t>
         </is>
@@ -2032,10 +2032,10 @@
       <c r="C77" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 0 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*D)[i] = (1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3];
-    (*C)[i] = ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + ((1 * (*D)[i - 1] + 1 * (*D)[i - 2]) + (*D)[i - 3]);
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*A)[i] = (*A)[i - 3] + ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*D)[i] = ((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3];
+    (*C)[i] = (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + (((*D)[i - 1] + (*D)[i - 2]) + (*D)[i - 3]);
+    (*B)[i] = (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
   }
 </t>
         </is>
@@ -2053,10 +2053,10 @@
       <c r="C78" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*A)[i] = ((0 * (*A)[i - 1] + 2 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
+    (*A)[i] = (2 * (*A)[i - 2] + (*A)[i - 3]) + ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
     (*D)[i] = (2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
-    (*B)[i] = ((1 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*C)[i] = ((1 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + ((1 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*B)[i] = (((*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]);
+    (*C)[i] = (((*C)[i - 1] + 2 * (*C)[i - 2]) + (*C)[i - 3]) + (((*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
   }
 </t>
         </is>
@@ -2074,9 +2074,9 @@
       <c r="C79" t="inlineStr">
         <is>
           <t xml:space="preserve">  for (int i = 3; i &lt;= (size - 1) / n_arrs; i += 1) {
-    (*B)[i] = ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]);
-    (*A)[i] = ((2 * (*A)[i - 1] + 1 * (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + 1 * (*B)[i - 2]) + (*B)[i - 3]);
-    (*C)[i] = ((2 * (*C)[i - 1] + 1 * (*C)[i - 2]) + (*C)[i - 3]) + ((2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
+    (*B)[i] = ((2 * (*B)[i - 1] + 2 * (*B)[i - 2]) + (*B)[i - 3]) + ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]);
+    (*A)[i] = ((2 * (*A)[i - 1] + (*A)[i - 2]) + (*A)[i - 3]) + ((2 * (*B)[i - 1] + (*B)[i - 2]) + (*B)[i - 3]);
+    (*C)[i] = ((2 * (*C)[i - 1] + (*C)[i - 2]) + (*C)[i - 3]) + ((2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3]);
     (*D)[i] = (2 * (*D)[i - 1] + 2 * (*D)[i - 2]) + (*D)[i - 3];
   }
 </t>

</xml_diff>